<commit_message>
Add the xlsx file handler on server side. Module xlsx is added to dependencies.
</commit_message>
<xml_diff>
--- a/example_data/analyses.xlsx
+++ b/example_data/analyses.xlsx
@@ -8,14 +8,15 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="123" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuille1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="hoho" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="haha" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="80">
   <si>
     <t>analyse_ID</t>
   </si>
@@ -240,6 +241,21 @@
   </si>
   <si>
     <t>Vivent les marmottes</t>
+  </si>
+  <si>
+    <t>toto</t>
+  </si>
+  <si>
+    <t>titi</t>
+  </si>
+  <si>
+    <t>tata</t>
+  </si>
+  <si>
+    <t>poisson</t>
+  </si>
+  <si>
+    <t>mercredi</t>
   </si>
 </sst>
 </file>
@@ -353,7 +369,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -689,4 +705,75 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add cast function on client and server sides to handle the uploaded data. Dates are not currently supported, only integers, floats, booleans and strings.
</commit_message>
<xml_diff>
--- a/example_data/analyses.xlsx
+++ b/example_data/analyses.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="70">
   <si>
     <t>analyse_ID</t>
   </si>
@@ -48,141 +48,120 @@
     <t>20140926_AN_Blanc2</t>
   </si>
   <si>
+    <t>file1</t>
+  </si>
+  <si>
+    <t>2015-01-01</t>
+  </si>
+  <si>
+    <t>strain1</t>
+  </si>
+  <si>
+    <t>blabla</t>
+  </si>
+  <si>
+    <t>BY4741_HCHO_F4</t>
+  </si>
+  <si>
+    <t>20140926_AN_LD_BY4741_HCHO_GradPoly_F4</t>
+  </si>
+  <si>
+    <t>file2</t>
+  </si>
+  <si>
+    <t>2015-02-02</t>
+  </si>
+  <si>
+    <t>blablablabla</t>
+  </si>
+  <si>
+    <t>BL3</t>
+  </si>
+  <si>
+    <t>20140926_AN_Blanc3</t>
+  </si>
+  <si>
+    <t>file3</t>
+  </si>
+  <si>
+    <t>2015-03-03</t>
+  </si>
+  <si>
+    <t>hoho</t>
+  </si>
+  <si>
+    <t>BY4741_HCHO_F6</t>
+  </si>
+  <si>
+    <t>20140926_AN_LD_BY4741_HCHO_GradPoly_F6</t>
+  </si>
+  <si>
+    <t>file4</t>
+  </si>
+  <si>
+    <t>2015-04-04</t>
+  </si>
+  <si>
+    <t>haha</t>
+  </si>
+  <si>
+    <t>BL4</t>
+  </si>
+  <si>
+    <t>20140926_AN_Blanc4</t>
+  </si>
+  <si>
+    <t>file5</t>
+  </si>
+  <si>
+    <t>2015-05-05</t>
+  </si>
+  <si>
+    <t>hihi</t>
+  </si>
+  <si>
+    <t>BY4741_HCHO_F9</t>
+  </si>
+  <si>
+    <t>20140926_AN_LD_BY4741_HCHO_GradPoly_F9</t>
+  </si>
+  <si>
+    <t>file6</t>
+  </si>
+  <si>
+    <t>2015-06-06</t>
+  </si>
+  <si>
+    <t>Je suis une fougère</t>
+  </si>
+  <si>
+    <t>BL5</t>
+  </si>
+  <si>
+    <t>20140926_AN_Blanc5</t>
+  </si>
+  <si>
+    <t>file7</t>
+  </si>
+  <si>
+    <t>2015-07-07</t>
+  </si>
+  <si>
+    <t>Why so serious ?</t>
+  </si>
+  <si>
+    <t>BY4741_HCHO_F10</t>
+  </si>
+  <si>
+    <t>20140926_AN_LD_BY4741_HCHO_GradPoly_F10</t>
+  </si>
+  <si>
+    <t>file8</t>
+  </si>
+  <si>
     <t>2015-08-08</t>
   </si>
   <si>
-    <t>file1</t>
-  </si>
-  <si>
-    <t>2015-01-01</t>
-  </si>
-  <si>
-    <t>strain1</t>
-  </si>
-  <si>
-    <t>blabla</t>
-  </si>
-  <si>
-    <t>BY4741_HCHO_F4</t>
-  </si>
-  <si>
-    <t>20140926_AN_LD_BY4741_HCHO_GradPoly_F4</t>
-  </si>
-  <si>
-    <t>2015-08-09</t>
-  </si>
-  <si>
-    <t>file2</t>
-  </si>
-  <si>
-    <t>2015-02-02</t>
-  </si>
-  <si>
-    <t>blablablabla</t>
-  </si>
-  <si>
-    <t>BL3</t>
-  </si>
-  <si>
-    <t>20140926_AN_Blanc3</t>
-  </si>
-  <si>
-    <t>2015-08-10</t>
-  </si>
-  <si>
-    <t>file3</t>
-  </si>
-  <si>
-    <t>2015-03-03</t>
-  </si>
-  <si>
-    <t>hoho</t>
-  </si>
-  <si>
-    <t>BY4741_HCHO_F6</t>
-  </si>
-  <si>
-    <t>20140926_AN_LD_BY4741_HCHO_GradPoly_F6</t>
-  </si>
-  <si>
-    <t>2015-08-11</t>
-  </si>
-  <si>
-    <t>file4</t>
-  </si>
-  <si>
-    <t>2015-04-04</t>
-  </si>
-  <si>
-    <t>haha</t>
-  </si>
-  <si>
-    <t>BL4</t>
-  </si>
-  <si>
-    <t>20140926_AN_Blanc4</t>
-  </si>
-  <si>
-    <t>2015-08-12</t>
-  </si>
-  <si>
-    <t>file5</t>
-  </si>
-  <si>
-    <t>2015-05-05</t>
-  </si>
-  <si>
-    <t>hihi</t>
-  </si>
-  <si>
-    <t>BY4741_HCHO_F9</t>
-  </si>
-  <si>
-    <t>20140926_AN_LD_BY4741_HCHO_GradPoly_F9</t>
-  </si>
-  <si>
-    <t>2015-08-13</t>
-  </si>
-  <si>
-    <t>file6</t>
-  </si>
-  <si>
-    <t>2015-06-06</t>
-  </si>
-  <si>
-    <t>Je suis une fougère</t>
-  </si>
-  <si>
-    <t>BL5</t>
-  </si>
-  <si>
-    <t>20140926_AN_Blanc5</t>
-  </si>
-  <si>
-    <t>2015-08-14</t>
-  </si>
-  <si>
-    <t>file7</t>
-  </si>
-  <si>
-    <t>2015-07-07</t>
-  </si>
-  <si>
-    <t>Why so serious ?</t>
-  </si>
-  <si>
-    <t>BY4741_HCHO_F10</t>
-  </si>
-  <si>
-    <t>20140926_AN_LD_BY4741_HCHO_GradPoly_F10</t>
-  </si>
-  <si>
-    <t>2015-08-15</t>
-  </si>
-  <si>
-    <t>file8</t>
-  </si>
-  <si>
     <t>strain2</t>
   </si>
   <si>
@@ -195,9 +174,6 @@
     <t>20140926_AN_Blanc6</t>
   </si>
   <si>
-    <t>2015-08-16</t>
-  </si>
-  <si>
     <t>file9</t>
   </si>
   <si>
@@ -213,9 +189,6 @@
     <t>20140926_AN_LD_BY4741_HCHO_GradPoly_F15</t>
   </si>
   <si>
-    <t>2015-08-17</t>
-  </si>
-  <si>
     <t>file10</t>
   </si>
   <si>
@@ -229,9 +202,6 @@
   </si>
   <si>
     <t>20140926_AN_Blanc7</t>
-  </si>
-  <si>
-    <t>2015-08-18</t>
   </si>
   <si>
     <t>file11</t>
@@ -369,7 +339,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -420,280 +390,280 @@
       <c r="C2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="1" t="n">
+        <v>42224</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>42225</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="G3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>42226</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="G4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>42227</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>5</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>42228</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>42229</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>7</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>41500</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>42231</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>9</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>41867</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>10</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>42233</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>11</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>42234</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -725,13 +695,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -747,13 +717,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>